<commit_message>
update question submission message
</commit_message>
<xml_diff>
--- a/Questions English.xlsx
+++ b/Questions English.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chloe\Documents\GitHub\Game-Teacher-Admin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B235A31B-FE04-4280-B8F1-697FC4EAD56F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{464B0BE3-8897-450A-B805-AB68DD6C0585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{36722717-C41C-43F9-8F72-24C2463940E3}"/>
+    <workbookView xWindow="4932" yWindow="1560" windowWidth="17280" windowHeight="10392" xr2:uid="{36722717-C41C-43F9-8F72-24C2463940E3}"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="2" r:id="rId1"/>
@@ -897,7 +897,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>